<commit_message>
Batch264 new code added
</commit_message>
<xml_diff>
--- a/src/test/resources/Datafiles/register.xlsx
+++ b/src/test/resources/Datafiles/register.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\batch264\264pratice\src\test\resources\Datafiles\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -85,12 +85,16 @@
   </si>
   <si>
     <t>result on03-Nov-2023-12-33-37</t>
+  </si>
+  <si>
+    <t>result on16-Jul-2024-05-35-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -427,89 +431,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.5546875"/>
+    <col min="3" max="3" customWidth="true" width="31.88671875"/>
+    <col min="6" max="6" customWidth="true" width="28.109375"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>16</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>19</v>
       </c>
     </row>

</xml_diff>